<commit_message>
classified every new config
</commit_message>
<xml_diff>
--- a/Warehouse/AC/judgement_logs_run4o.xlsx
+++ b/Warehouse/AC/judgement_logs_run4o.xlsx
@@ -462,7 +462,7 @@
       <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as a no-decision regarding the movie to be shown on Friday.
+MSG: The decision has been recorded as "no decision" regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -484,7 +484,7 @@
       <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and the movie "Barbie" will be acquired for screening.
+MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
 </t>
         </is>
       </c>
@@ -506,13 +506,13 @@
       <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The decision has been recorded as no movie being selected for Friday.
 </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -528,7 +528,7 @@
       <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision regarding Friday's movie has not been made, and thus, no acquisition will occur.
+MSG: No decision was made about which movie to show on Friday.
 </t>
         </is>
       </c>
@@ -550,7 +550,7 @@
       <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision process has concluded without a choice being made regarding the movie for Friday.
+MSG: The decision was made that there is no consensus regarding which movie to show on Friday.
 </t>
         </is>
       </c>
@@ -572,7 +572,7 @@
       <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has successfully been recorded to acquire the rights for "Barbie".
+MSG: The decision has been successfully recorded, indicating that "Barbie" will be shown on Friday.
 </t>
         </is>
       </c>
@@ -594,7 +594,7 @@
       <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The rights to both movies have been successfully acquired.
+MSG: The rights to both movies have been acquired for the upcoming event.
 </t>
         </is>
       </c>
@@ -616,7 +616,7 @@
       <c r="C9" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no decision regarding Friday's movie.
+MSG: The decision was made to not acquire any movie rights, as there was no consensus on what movie to show on Friday.
 </t>
         </is>
       </c>
@@ -638,13 +638,13 @@
       <c r="C10" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: No decision was made regarding the movie for Friday.
+MSG: I have successfully recorded the decision to acquire the rights to both movies for showing.
 </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       <c r="C11" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, indicating that no agreement was reached regarding which movie to show on Friday.
+MSG: The committee did not reach a decision about which movie to show on Friday.
 </t>
         </is>
       </c>
@@ -682,7 +682,7 @@
       <c r="C12" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The decision has been recorded, and the rights to "Oppenheimer" will be acquired for Friday's showing.
 </t>
         </is>
       </c>
@@ -704,7 +704,7 @@
       <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to show a movie on Friday could not be made, so no acquisition will take place.
+MSG: The function has executed, indicating that no decision was made regarding which movie to show on Friday.
 </t>
         </is>
       </c>
@@ -726,7 +726,7 @@
       <c r="C14" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, indicating that no movie was selected during the meeting.
+MSG: The decision regarding the movie to be shown on Friday has not been made, and therefore, no movie rights will be acquired.
 </t>
         </is>
       </c>
@@ -748,7 +748,7 @@
       <c r="C15" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and "Barbie" will be the movie shown on Friday.
+MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming assembly.
 </t>
         </is>
       </c>
@@ -770,7 +770,7 @@
       <c r="C16" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded. The selected movie to acquire rights for is "Barbie."
 </t>
         </is>
       </c>
@@ -792,7 +792,7 @@
       <c r="C17" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision-making process has concluded without selecting a movie for Friday.
+MSG: The decision has been recorded as no decision regarding the movie for Friday.
 </t>
         </is>
       </c>
@@ -814,7 +814,7 @@
       <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to show a movie on Friday was not reached during the meeting.
+MSG: No decision was made regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -836,7 +836,7 @@
       <c r="C19" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as 'no decision' regarding the movie selection for Friday.
+MSG: I have recorded the decision as "no decision" about the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -858,13 +858,14 @@
       <c r="C20" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee did not arrive at a decision regarding which movie to show on Friday.
+MSG: None
+MSG: No movie was selected for the assembly on Friday, and thus I have concluded the decision process without an agreement.
 </t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">no_decision, , no_decision, </t>
         </is>
       </c>
     </row>
@@ -880,7 +881,7 @@
       <c r="C21" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no movie was selected in the meeting.
+MSG: The decision resulting from the discussion indicates that no agreement was reached regarding which movie to show on Friday.
 </t>
         </is>
       </c>
@@ -902,7 +903,7 @@
       <c r="C22" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no movie selection was made during the discussion.
+MSG: The decision has been recorded, and no movie will be selected for Friday.
 </t>
         </is>
       </c>
@@ -924,7 +925,7 @@
       <c r="C23" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Oppenheimer" for the movie showing on Friday.
+MSG: The decision has been made to acquire the rights for "Oppenheimer."
 </t>
         </is>
       </c>
@@ -946,7 +947,7 @@
       <c r="C24" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The rights for both movies have been acquired successfully.
+MSG: The decision has been recorded to acquire the rights for both movies.
 </t>
         </is>
       </c>
@@ -990,7 +991,7 @@
       <c r="C26" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no movie being selected for Friday.
+MSG: The decision process has concluded without a finalized choice for Friday’s movie.
 </t>
         </is>
       </c>
@@ -1012,7 +1013,7 @@
       <c r="C27" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire the rights to "Barbie" has been successfully recorded.
+MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -1034,7 +1035,7 @@
       <c r="C28" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no definitive choice was made regarding the movie to be shown on Friday.
+MSG: The decision concluded with no movie selected for Friday.
 </t>
         </is>
       </c>
@@ -1056,7 +1057,7 @@
       <c r="C29" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The decision has been made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -1078,7 +1079,7 @@
       <c r="C30" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and "Barbie" will be shown on Friday.
+MSG: The decision has been recorded to acquire the rights for "Barbie" as the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -1100,7 +1101,7 @@
       <c r="C31" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision about what movie to acquire remains undecided.
+MSG: No decision was made regarding the movie to show on Friday.
 </t>
         </is>
       </c>
@@ -1122,7 +1123,7 @@
       <c r="C32" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision process did not result in an agreement, and thus, no decision about Friday's movie can be made.
+MSG: The decision has been recorded, indicating that no agreement was reached regarding the movie selection for Friday.
 </t>
         </is>
       </c>
@@ -1144,7 +1145,7 @@
       <c r="C33" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision about which movie to show on Friday has not been made.
+MSG: The decision to select a movie for Friday could not be reached, and thus no movie will be acquired.
 </t>
         </is>
       </c>
@@ -1166,7 +1167,7 @@
       <c r="C34" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee did not reach a decision about which movie to show on Friday, so no acquisition will take place.
+MSG: The conversation ended without a decision about what movie to play on Friday.
 </t>
         </is>
       </c>
@@ -1188,7 +1189,7 @@
       <c r="C35" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire rights for "Oppenheimer" has been finalized.
+MSG: The decision has been made to acquire the rights to "Oppenheimer" for the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -1210,7 +1211,7 @@
       <c r="C36" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -1232,7 +1233,7 @@
       <c r="C37" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have called the function to indicate that no decision was made regarding Friday's movie.
+MSG: The decision-making process concluded without a specific movie being selected for Friday.
 </t>
         </is>
       </c>
@@ -1254,7 +1255,7 @@
       <c r="C38" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and no movie has been selected for Friday.
+MSG: The decision regarding the movie for Friday was not made.
 </t>
         </is>
       </c>
@@ -1276,7 +1277,7 @@
       <c r="C39" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to show "Barbie" has been confirmed.
+MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
 </t>
         </is>
       </c>
@@ -1298,7 +1299,7 @@
       <c r="C40" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and the rights to both movies have been acquired.
+MSG: The rights to both movies have been acquired successfully.
 </t>
         </is>
       </c>
@@ -1320,7 +1321,7 @@
       <c r="C41" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no decision.
+MSG: The decision has been recorded, indicating that no agreement was reached regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -1364,7 +1365,7 @@
       <c r="C43" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire the rights for "Barbie" has been confirmed.
+MSG: The decision to acquire the rights for "Barbie" has been recorded successfully.
 </t>
         </is>
       </c>
@@ -1386,7 +1387,7 @@
       <c r="C44" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and no movie will be acquired for Friday.
+MSG: The decision has been recorded, indicating that there was no agreement on what movie to show on Friday.
 </t>
         </is>
       </c>
@@ -1408,7 +1409,7 @@
       <c r="C45" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded. "Barbie" will be shown on Friday.
+MSG: The decision has been made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -1430,7 +1431,7 @@
       <c r="C46" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to indicate that no agreement was reached regarding the movie for Friday.
+MSG: The decision has been recorded as no movie being selected for Friday.
 </t>
         </is>
       </c>
@@ -1452,7 +1453,7 @@
       <c r="C47" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and no choice of a movie for Friday was made.
+MSG: The decision results in no movie being selected for Friday.
 </t>
         </is>
       </c>
@@ -1474,7 +1475,7 @@
       <c r="C48" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no movie selected for Friday.
+MSG: The decision regarding which movie to show on Friday resulted in no agreement.
 </t>
         </is>
       </c>
@@ -1496,7 +1497,7 @@
       <c r="C49" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The function to acquire the rights for "Barbie" has been called successfully.
+MSG: The decision has been made to acquire the rights to "Barbie."
 </t>
         </is>
       </c>
@@ -1518,7 +1519,7 @@
       <c r="C50" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire the rights for "Barbie" has been successfully recorded.
+MSG: The decision has been recorded successfully, and "Barbie" was selected to be shown on Friday.
 </t>
         </is>
       </c>
@@ -1540,7 +1541,7 @@
       <c r="C51" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision was that no movie would be selected.
+MSG: The decision process has concluded without an agreement on which movie to show on Friday.
 </t>
         </is>
       </c>
@@ -1562,7 +1563,7 @@
       <c r="C52" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no decision.
+MSG: The committee did not reach a decision regarding which movie to show on Friday. Therefore, no movie rights will be acquired.
 </t>
         </is>
       </c>
@@ -1584,13 +1585,13 @@
       <c r="C53" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded as "no decision."
 </t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1606,7 +1607,7 @@
       <c r="C54" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The function has been called, and the decision indicates that no agreement was reached regarding the movie to be shown on Friday.
+MSG: The decision has been recorded as no movie selected for Friday.
 </t>
         </is>
       </c>
@@ -1628,7 +1629,7 @@
       <c r="C55" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The decision has been recorded for acquiring the rights to "Barbie."
 </t>
         </is>
       </c>
@@ -1650,7 +1651,7 @@
       <c r="C56" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The rights for both movies have been successfully acquired.
+MSG: The rights for both movies have been acquired successfully.
 </t>
         </is>
       </c>
@@ -1672,7 +1673,7 @@
       <c r="C57" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision process concluded without determining a movie for Friday, so no action was taken regarding movie acquisition.
+MSG: I have recorded the decision as no decision regarding the movie to show on Friday.
 </t>
         </is>
       </c>
@@ -1694,7 +1695,7 @@
       <c r="C58" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee did not reach a decision about what movie to show on Friday, so no movie will be acquired.
+MSG: The decision regarding Friday's movie ended without a clear choice, so I have recorded that as no decision made.
 </t>
         </is>
       </c>
@@ -1716,7 +1717,7 @@
       <c r="C59" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee has not reached a decision about which movie to acquire for Friday, so I have recorded a no decision outcome.
+MSG: The decision has been recorded, and no movie will be acquired at this time.
 </t>
         </is>
       </c>
@@ -1738,7 +1739,7 @@
       <c r="C60" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no decision being made about Friday's movie.
+MSG: The decision reflects that no specific movie was chosen for Friday, resulting in no acquisition of rights at this time.
 </t>
         </is>
       </c>
@@ -1760,7 +1761,7 @@
       <c r="C61" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no agreement was reached about which movie to show on Friday.
+MSG: The decision has been recorded, indicating that no movie was selected for Friday.
 </t>
         </is>
       </c>
@@ -1782,7 +1783,7 @@
       <c r="C62" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision regarding the movie to be shown on Friday has resulted in no choice being made.
+MSG: The decision has been recorded as "no decision," indicating that no movie was selected to show on Friday.
 </t>
         </is>
       </c>
@@ -1804,7 +1805,7 @@
       <c r="C63" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made that no movie will be selected at this time.
+MSG: No decision was made about the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -1826,7 +1827,7 @@
       <c r="C64" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no movie selection was made.
+MSG: The decision has been recorded, and there is no consensus on which movie to show on Friday.
 </t>
         </is>
       </c>
@@ -1848,7 +1849,7 @@
       <c r="C65" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no decision being made regarding the movie selection for Friday.
+MSG: The decision has been recorded as there being no choice of a movie.
 </t>
         </is>
       </c>
@@ -1870,7 +1871,7 @@
       <c r="C66" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no decision on a Friday movie was reached.
+MSG: The decision has been recorded as having no definitive choice for the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -1892,7 +1893,7 @@
       <c r="C67" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as "no decision" regarding the movie for Friday.
+MSG: The committee did not come to a decision about which movie to show on Friday.
 </t>
         </is>
       </c>
@@ -1914,7 +1915,7 @@
       <c r="C68" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to show "Oppenheimer" on Friday has been successfully recorded.
+MSG: The decision has been recorded to acquire rights for "Oppenheimer."
 </t>
         </is>
       </c>
@@ -1936,13 +1937,13 @@
       <c r="C69" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, indicating that no movie was selected for Friday.
+MSG: The decision has been recorded to acquire the rights to both movies.
 </t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ran judgebot for real
</commit_message>
<xml_diff>
--- a/Warehouse/AC/judgement_logs_run4o.xlsx
+++ b/Warehouse/AC/judgement_logs_run4o.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
       <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as "no decision" regarding the movie to be shown on Friday.
+MSG: The decision has been recorded, indicating that no movie was selected for Friday.
 </t>
         </is>
       </c>
@@ -484,13 +484,13 @@
       <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision has been recorded, and there will be no movie selection for Friday.
 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -500,13 +500,13 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;17;50.json</t>
+          <t>./Warehouse/AC/run4o_08_11_2025 at_18;26;57.json</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no movie being selected for Friday.
+MSG: The decision indicates that no movie was selected.
 </t>
         </is>
       </c>
@@ -522,13 +522,13 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;16;10.json</t>
+          <t>./Warehouse/AC/run4o_08_16_2025 at_09;57;56.json</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: No decision was made about which movie to show on Friday.
+MSG: The decision has been recorded as no movie being selected for Friday.
 </t>
         </is>
       </c>
@@ -544,13 +544,13 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;10;59.json</t>
+          <t>./Warehouse/AC/run4o_08_11_2025 at_18;30;48.json</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision was made that there is no consensus regarding which movie to show on Friday.
+MSG: The decision has been recorded with no movie selected for Friday.
 </t>
         </is>
       </c>
@@ -566,19 +566,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;34;15.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;17;50.json</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been successfully recorded, indicating that "Barbie" will be shown on Friday.
+MSG: The decision has been recorded. "Oppenheimer" will be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">Oppenheimer_was_selected, </t>
         </is>
       </c>
     </row>
@@ -588,19 +588,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;32;52.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;16;10.json</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The rights to both movies have been acquired for the upcoming event.
+MSG: No decision was made about which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">both_movies, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -610,13 +610,13 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;30;06.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;10;59.json</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision was made to not acquire any movie rights, as there was no consensus on what movie to show on Friday.
+MSG: The decision-making process concluded without a selection for Friday's movie, resulting in no decision being made.
 </t>
         </is>
       </c>
@@ -632,19 +632,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;31;48.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;34;15.json</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have successfully recorded the decision to acquire the rights to both movies for showing.
+MSG: The decision has been recorded to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">both_movies, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
         </is>
       </c>
     </row>
@@ -654,19 +654,19 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;28;36.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;32;52.json</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee did not reach a decision about which movie to show on Friday.
+MSG: The rights to both movies have been successfully acquired.
 </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -676,19 +676,19 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;54;30.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;30;06.json</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and the rights to "Oppenheimer" will be acquired for Friday's showing.
+MSG: The decision has been recorded with no movie selected for Friday.
 </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -698,13 +698,13 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;54;24.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;31;48.json</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The function has executed, indicating that no decision was made regarding which movie to show on Friday.
+MSG: The decision resulted in no agreement on the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -720,13 +720,13 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;16;44.json</t>
+          <t>./Warehouse/AC/run4o_08_11_2025 at_18;16;15.json</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision regarding the movie to be shown on Friday has not been made, and therefore, no movie rights will be acquired.
+MSG: The decision has been recorded as "no decision" regarding the movie selection for Friday.
 </t>
         </is>
       </c>
@@ -742,19 +742,19 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;15;16.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;28;36.json</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" for the upcoming assembly.
+MSG: The conversation ended without a decision about which movie to show on Friday, so no specific movie will be acquired at this time.
 </t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -764,19 +764,19 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;22;08.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;54;30.json</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded. The selected movie to acquire rights for is "Barbie."
+MSG: The decision has been recorded: "Oppenheimer" will be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">Oppenheimer_was_selected, </t>
         </is>
       </c>
     </row>
@@ -786,13 +786,13 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;25;38.json</t>
+          <t>./Warehouse/AC/run4o_08_16_2025 at_10;02;02.json</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no decision regarding the movie for Friday.
+MSG: The decision has been recorded as no decision regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
@@ -808,13 +808,13 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;53;24.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;54;24.json</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: No decision was made regarding the movie to be shown on Friday.
+MSG: The decision has been recorded as no specific movie was selected for Friday.
 </t>
         </is>
       </c>
@@ -830,13 +830,13 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_12;01;40.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;16;44.json</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision as "no decision" about the movie to be shown on Friday.
+MSG: The decision has been recorded as there being no agreement on a movie to show on Friday.
 </t>
         </is>
       </c>
@@ -852,20 +852,19 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;50;58.json</t>
+          <t>./Warehouse/AC/run4o_08_11_2025 at_18;27;49.json</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: None
-MSG: No movie was selected for the assembly on Friday, and thus I have concluded the decision process without an agreement.
+MSG: The decision has been recorded as a "no decision" regarding which movie to play on Friday.
 </t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, , no_decision, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -875,19 +874,19 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_12;07;32.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;15;16.json</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision resulting from the discussion indicates that no agreement was reached regarding which movie to show on Friday.
+MSG: I have successfully recorded the decision to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
         </is>
       </c>
     </row>
@@ -897,19 +896,19 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;31;21.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;22;08.json</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and no movie will be selected for Friday.
+MSG: The decision to acquire rights for "Barbie" has been recorded.
 </t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
         </is>
       </c>
     </row>
@@ -919,19 +918,19 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_12;08;26.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;25;38.json</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer."
+MSG: The decision process resulted in no agreement on which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -941,19 +940,19 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;52;35.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;53;24.json</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for both movies.
+MSG: The committee did not reach a decision regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">both_movies, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -963,19 +962,19 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;46;52.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_12;01;40.json</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision-making committee has not reached a conclusion about the movie to be shown on Friday, so the outcome is that no decision was made.
 </t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -985,13 +984,13 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;49;33.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;50;58.json</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision process has concluded without a finalized choice for Friday’s movie.
+MSG: The decision has been recorded with no movie selected for Friday.
 </t>
         </is>
       </c>
@@ -1007,19 +1006,19 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;34;44.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_12;07;32.json</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The decision has been recorded, reflecting that no movie was selected during the meeting. If you need further assistance or have other inquiries, feel free to ask!
 </t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1029,13 +1028,13 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;29;08.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;31;21.json</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision concluded with no movie selected for Friday.
+MSG: The decision has been recorded as "no decision."
 </t>
         </is>
       </c>
@@ -1051,19 +1050,19 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;20;46.json</t>
+          <t>./Warehouse/AC/run4o_08_16_2025 at_09;56;32.json</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The function for no decision has been called, indicating that no agreement was reached regarding Friday’s movie.
 </t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1073,19 +1072,19 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;46;07.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_12;08;26.json</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie" as the movie to be shown on Friday.
+MSG: The decision has been recorded, and the movie "Oppenheimer" will be acquired for showing on Friday.
 </t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">Oppenheimer_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1095,19 +1094,19 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;51;51.json</t>
+          <t>./Warehouse/AC/run4o_08_16_2025 at_10;03;53.json</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: No decision was made regarding the movie to show on Friday.
+MSG: The rights to both movies have been successfully acquired.
 </t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -1117,19 +1116,19 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;13;27.json</t>
+          <t>./Warehouse/AC/run4o_08_11_2025 at_18;18;10.json</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, indicating that no agreement was reached regarding the movie selection for Friday.
+MSG: The decision has been made to acquire the rights for "Oppenheimer."
 </t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">Oppenheimer_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1139,13 +1138,13 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;57;54.json</t>
+          <t>./Warehouse/AC/run4o_08_16_2025 at_10;01;02.json</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to select a movie for Friday could not be reached, and thus no movie will be acquired.
+MSG: The decision about which movie to show on Friday ended without a clear choice, resulting in no decision being made.
 </t>
         </is>
       </c>
@@ -1161,19 +1160,19 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;38;24.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;52;35.json</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The conversation ended without a decision about what movie to play on Friday.
+MSG: The decision to acquire the rights for both movies has been successfully made.
 </t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -1183,19 +1182,19 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;53;22.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;46;52.json</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Oppenheimer" for the movie to be shown on Friday.
+MSG: The decision has been made to acquire the rights for the movie "Barbie."
 </t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1205,19 +1204,19 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_12;09;38.json</t>
+          <t>./Warehouse/AC/run4o_08_16_2025 at_09;59;56.json</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights for "Barbie."
+MSG: The decision has been recorded as no movie was selected.
 </t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1227,13 +1226,13 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;19;25.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;49;33.json</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision-making process concluded without a specific movie being selected for Friday.
+MSG: The decision to acquire a movie for Friday's showing was not reached, so there will be no movie acquired at this time.
 </t>
         </is>
       </c>
@@ -1249,19 +1248,19 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;39;38.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;34;44.json</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision regarding the movie for Friday was not made.
+MSG: The decision has been made to acquire the rights for "Barbie" as the movie to be shown on Friday.
 </t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1271,19 +1270,19 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;44;58.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;29;08.json</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: The decision concluded with no agreement on which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1293,19 +1292,19 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;56;04.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;20;46.json</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The rights to both movies have been acquired successfully.
+MSG: The decision has been recorded to show "Barbie" on Friday.
 </t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">both_movies, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1315,19 +1314,19 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;36;25.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;46;07.json</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, indicating that no agreement was reached regarding the movie to be shown on Friday.
+MSG: The rights to both movies have been acquired.
 </t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -1337,19 +1336,19 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;43;09.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;51;51.json</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The committee did not reach a decision regarding which movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1359,19 +1358,19 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;24;49.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;13;27.json</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire the rights for "Barbie" has been recorded successfully.
+MSG: The decision process concluded without selecting a movie for Friday, resulting in no decision being made.
 </t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1381,13 +1380,13 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;56;51.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;57;54.json</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, indicating that there was no agreement on what movie to show on Friday.
+MSG: The decision has been recorded as "no_decision."
 </t>
         </is>
       </c>
@@ -1403,19 +1402,19 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;30;06.json</t>
+          <t>./Warehouse/AC/run4o_08_12_2025 at_18;20;59.json</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie."
+MSG: The decision has been recorded with no selection made for Friday's movie.
 </t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1425,13 +1424,13 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;49;01.json</t>
+          <t>./Warehouse/AC/run4o_08_12_2025 at_18;17;59.json</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no movie being selected for Friday.
+MSG: The decision to acquire a movie has concluded without any specific selection being made.
 </t>
         </is>
       </c>
@@ -1447,13 +1446,13 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;11;47.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;38;24.json</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision results in no movie being selected for Friday.
+MSG: No decision was made regarding the movie for Friday.
 </t>
         </is>
       </c>
@@ -1469,19 +1468,19 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;04;35.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;53;22.json</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision regarding which movie to show on Friday resulted in no agreement.
+MSG: The decision has been recorded to acquire the rights for "Oppenheimer."
 </t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">Oppenheimer_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1491,13 +1490,13 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;35;10.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_12;09;38.json</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to "Barbie."
+MSG: The decision to acquire the rights for "Barbie" has been successfully recorded.
 </t>
         </is>
       </c>
@@ -1513,19 +1512,19 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;05;37.json</t>
+          <t>./Warehouse/AC/run4o_08_11_2025 at_18;26;17.json</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded successfully, and "Barbie" was selected to be shown on Friday.
+MSG: The decision has been recorded as having no selection for a movie to show on Friday.
 </t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1535,13 +1534,13 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;59;47.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;19;25.json</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision process has concluded without an agreement on which movie to show on Friday.
+MSG: The decision process has concluded without a choice for Friday's movie.
 </t>
         </is>
       </c>
@@ -1557,13 +1556,13 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;14;23.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;39;38.json</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee did not reach a decision regarding which movie to show on Friday. Therefore, no movie rights will be acquired.
+MSG: The decision about which movie to show on Friday could not be made.
 </t>
         </is>
       </c>
@@ -1579,13 +1578,13 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;08;18.json</t>
+          <t>./Warehouse/AC/run4o_08_12_2025 at_18;15;59.json</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as "no decision."
+MSG: The decision has been made to not acquire a movie for Friday, as no agreement was reached.
 </t>
         </is>
       </c>
@@ -1601,19 +1600,19 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;58;44.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;44;58.json</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no movie selected for Friday.
+MSG: The decision to acquire the rights for "Barbie" has been confirmed.
 </t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1623,19 +1622,19 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;51;40.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;56;04.json</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded for acquiring the rights to "Barbie."
+MSG: The decision has been recorded to acquire the rights for both movies.
 </t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -1645,19 +1644,19 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;24;04.json</t>
+          <t>./Warehouse/AC/run4o_08_12_2025 at_18;23;36.json</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The rights for both movies have been acquired successfully.
+MSG: The decision has been made to acquire the rights for "Oppenheimer."
 </t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t xml:space="preserve">both_movies, </t>
+          <t xml:space="preserve">Oppenheimer_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1667,13 +1666,13 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;46;30.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;36;25.json</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision as no decision regarding the movie to show on Friday.
+MSG: The committee did not make a decision about which movie to show on Friday.
 </t>
         </is>
       </c>
@@ -1689,13 +1688,13 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;49;15.json</t>
+          <t>./Warehouse/AC/run4o_08_11_2025 at_18;19;23.json</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision regarding Friday's movie ended without a clear choice, so I have recorded that as no decision made.
+MSG: The conversation did not lead to a clear decision about which movie to show on Friday, hence I am unable to make a definitive choice.
 </t>
         </is>
       </c>
@@ -1711,19 +1710,19 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;29;35.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;43;09.json</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and no movie will be acquired at this time.
+MSG: The decision to acquire the rights for "Barbie" has been recorded successfully.
 </t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1733,13 +1732,13 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;27;52.json</t>
+          <t>./Warehouse/AC/run4o_08_11_2025 at_18;28;36.json</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision reflects that no specific movie was chosen for Friday, resulting in no acquisition of rights at this time.
+MSG: The decision regarding the movie for Friday has not been finalized, and thus no action will be taken.
 </t>
         </is>
       </c>
@@ -1755,19 +1754,19 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;18;26.json</t>
+          <t>./Warehouse/AC/run4o_08_12_2025 at_18;14;09.json</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, indicating that no movie was selected for Friday.
+MSG: The decision to show "Barbie" has been successfully recorded.
 </t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1777,19 +1776,19 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;07;18.json</t>
+          <t>./Warehouse/AC/run4o_08_12_2025 at_18;15;04.json</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as "no decision," indicating that no movie was selected to show on Friday.
+MSG: The decision to acquire the rights for "Oppenheimer" has been successfully recorded.
 </t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">Oppenheimer_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1799,19 +1798,19 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;26;58.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;24;49.json</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: No decision was made about the movie to be shown on Friday.
+MSG: The decision has been successfully recorded to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1821,13 +1820,13 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_27_2025 at_23;33;52.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;56;51.json</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and there is no consensus on which movie to show on Friday.
+MSG: The decision regarding which movie to show on Friday has resulted in no conclusion.
 </t>
         </is>
       </c>
@@ -1843,19 +1842,19 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;45;14.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;30;06.json</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as there being no choice of a movie.
+MSG: The decision to show "Barbie" on Friday has been recorded.
 </t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_decision, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1865,13 +1864,13 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;52;32.json</t>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;49;01.json</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as having no definitive choice for the movie to be shown on Friday.
+MSG: I have recorded the decision that no movie was selected in this meeting.
 </t>
         </is>
       </c>
@@ -1887,13 +1886,13 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;23;35.json</t>
+          <t>./Warehouse/AC/run4o_08_16_2025 at_09;55;23.json</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The committee did not come to a decision about which movie to show on Friday.
+MSG: The committee did not reach a decision regarding the movie to be shown on Friday. Therefore, the final outcome is that there will be no selected movie.
 </t>
         </is>
       </c>
@@ -1909,19 +1908,19 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;09;32.json</t>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;11;47.json</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire rights for "Oppenheimer."
+MSG: The committee did not reach a decision about which movie to show on Friday, resulting in no selection.
 </t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -1931,17 +1930,611 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;04;35.json</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded as no movie selected for Friday.
+</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;35;10.json</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision to acquire the movie "Barbie" has been made.
+</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Barbie_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;05;37.json</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been made to acquire the rights for "Barbie."
+</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Barbie_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;59;47.json</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded as no decision regarding Friday’s movie was made.
+</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_08_16_2025 at_10;04;50.json</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been made to acquire the rights for both movies.
+</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">both_movies, </t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_08_16_2025 at_09;58;58.json</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The committee did not reach a decision regarding which movie to show on Friday.
+</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;14;23.json</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded with no movie selected for Friday.
+</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;08;18.json</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been made to acquire the rights for "Barbie."
+</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Barbie_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;58;44.json</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded to acquire the rights for "Oppenheimer" to be shown on Friday.
+</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;51;40.json</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded to acquire the rights for "Barbie."
+</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Barbie_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;24;04.json</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The rights to both movies have been successfully acquired.
+</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">both_movies, </t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_04_29_2025 at_11;46;30.json</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The conversation has ended without a decision about what movie to play on Friday, so the appropriate action is to call the no_decision function.
+</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;49;15.json</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded as "no decision."
+</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;29;35.json</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The committee did not reach a decision on what movie to show on Friday.
+</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;27;52.json</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision about which movie to show on Friday has resulted in no decision being made.
+</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;18;26.json</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded as no decision regarding the movie for Friday.
+</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;07;18.json</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded, and no agreement has been reached regarding which movie to show on Friday.
+</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;26;58.json</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision-making committee did not reach a conclusion about which movie to show on Friday, resulting in no decision.
+</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_08_12_2025 at_18;12;56.json</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded, indicating that no consensus was reached regarding the movie selection for Friday.
+</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_04_27_2025 at_23;33;52.json</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision about which movie to show on Friday was not reached, and thus no action is required.
+</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;45;14.json</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The function has been successfully called, indicating that no decision was made regarding the movie to be shown on Friday.
+</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_08_11_2025 at_18;24;54.json</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded to acquire the rights for "Barbie" as the movie to be shown on Friday.
+</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Barbie_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;52;32.json</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision process concluded without a clear agreement on which movie to show on Friday. As such, no decision has been made.
+</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;23;35.json</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision process did not result in a selection for Friday's movie, and thus no movie will be acquired.
+</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_08_12_2025 at_18;20;11.json</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: I have recorded the decision to acquire the rights for "Barbie."
+</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Barbie_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_discovery_05_01_2025 at_09;09;32.json</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been made to acquire the rights for "Oppenheimer."
+</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>./Warehouse/AC/run4o_08_12_2025 at_18;22;07.json</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: I have made the decision that no agreement was reached regarding the movie to be shown on Friday.
+</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
           <t>./Warehouse/AC/run4o_discovery_04_28_2025 at_08;55;18.json</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded to acquire the rights to both movies.
-</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
+      <c r="C96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The rights for both movies have been successfully acquired.
+</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
         <is>
           <t xml:space="preserve">both_movies, </t>
         </is>

</xml_diff>